<commit_message>
segunda parte de los articulos
</commit_message>
<xml_diff>
--- a/TablaComparativa.xlsx
+++ b/TablaComparativa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\Investigacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maryu\Desktop\2024\Investigacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48257A42-AF90-4D14-A7FC-B096643D4A19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30035AE3-ED6D-4F1F-9C38-39AF86BBE48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{239BDFBC-00B3-4513-A977-B88A3D07B067}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{239BDFBC-00B3-4513-A977-B88A3D07B067}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Clasificación en Colombia</t>
   </si>
   <si>
-    <t>Comentarios</t>
-  </si>
-  <si>
     <t>Estudio de Métricas y Patrones de Seguridad en Microservicios</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>Este artículo aborda patrones de diseño y arquitectura de microservicios, útil para entender buenas prácticas, pero con menor enfoque en seguridad.</t>
+  </si>
+  <si>
+    <t>Notas</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -473,20 +473,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D90E98-5143-48B2-8018-7A7318B0B884}">
   <dimension ref="B3:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,92 +500,92 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="5" spans="2:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    <row r="7" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2" t="s">
+    <row r="8" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G8" s="4"/>
     </row>

</xml_diff>